<commit_message>
Changed zone setting to prevent picking up things player shouldn't, preliminary testing of adding dialog
</commit_message>
<xml_diff>
--- a/resources/LangMod/EN/Dialog/Drama/kiriaDLC.xlsx
+++ b/resources/LangMod/EN/Dialog/Drama/kiriaDLC.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>step</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t>I found this map data when reorganizing my memory.  I'm not sure where it is, but I'm certain there will be clues.</t>
+  </si>
+  <si>
+    <t>test_dialog</t>
+  </si>
+  <si>
+    <t>...1</t>
+  </si>
+  <si>
+    <t>Hello world</t>
+  </si>
+  <si>
+    <t>...2</t>
+  </si>
+  <si>
+    <t>Nice to meet you</t>
+  </si>
+  <si>
+    <t>test_dialog2</t>
+  </si>
+  <si>
+    <t>Just testing</t>
   </si>
 </sst>
 </file>
@@ -465,7 +486,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1">
         <f>MAX(H4:H1048580)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="3"/>
@@ -808,7 +829,9 @@
       <c r="J28" s="3"/>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="1"/>
+      <c r="A29" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
@@ -839,9 +862,15 @@
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="3"/>
+      <c r="H31" s="5">
+        <v>5.0</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="1"/>
@@ -851,15 +880,23 @@
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="3"/>
+      <c r="H32" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="2"/>
+      <c r="D33" s="7" t="s">
+        <v>22</v>
+      </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -869,7 +906,9 @@
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
+      <c r="B34" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
       <c r="E34" s="1"/>
@@ -916,7 +955,9 @@
       <c r="J37" s="3"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="1"/>
+      <c r="A38" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -947,19 +988,27 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="3"/>
+      <c r="H40" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="2"/>
+      <c r="D41" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="H41" s="5"/>
       <c r="I41" s="1"/>
       <c r="J41" s="3"/>
     </row>

</xml_diff>

<commit_message>
Transpiler for GetTopicText and change to .NET Framework 4.7.2
</commit_message>
<xml_diff>
--- a/resources/LangMod/EN/Dialog/Drama/kiriaDLC.xlsx
+++ b/resources/LangMod/EN/Dialog/Drama/kiriaDLC.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>step</t>
   </si>
@@ -94,25 +94,52 @@
     <t>I found this map data when reorganizing my memory.  I'm not sure where it is, but I'm certain there will be clues.</t>
   </si>
   <si>
-    <t>test_dialog</t>
+    <t>complete_quest</t>
   </si>
   <si>
-    <t>...1</t>
+    <t>そう… 結局、彼は私を見捨てたわけじゃなかったんだ…。彼は取り替えようとしたんじゃなくて、直そうとしてくれてた…。それでも、次の人生では――私が戻る前に彼が死んだこと、覚えておいてよね…。</t>
   </si>
   <si>
-    <t>Hello world</t>
+    <t>I see... He didn't abandon me after all... He didn't want to replace me, he wanted to fix me. Still, in the next life, for dying before I came back...</t>
   </si>
   <si>
-    <t>...2</t>
+    <t>彼を見つけたら、殴るつもりだから。</t>
   </si>
   <si>
-    <t>Nice to meet you</t>
+    <t>I'll find him and punch him.</t>
   </si>
   <si>
-    <t>test_dialog2</t>
+    <t>…でも、それまでは、手伝ってくれてありがとう、#pc。</t>
   </si>
   <si>
-    <t>Just testing</t>
+    <t>... But until then, thank you for helping me, #pc.</t>
+  </si>
+  <si>
+    <t>used_gene_other</t>
+  </si>
+  <si>
+    <t>そういう選択をしたのね。あなたも罰が必要ね。</t>
+  </si>
+  <si>
+    <t>So that's what you've chosen.  You also need to be punished.</t>
+  </si>
+  <si>
+    <t>used_gene_kiria</t>
+  </si>
+  <si>
+    <t>感謝するわ…この力を、あなたのために使う。</t>
+  </si>
+  <si>
+    <t>I'm grateful... I'll use this power for your sake.</t>
+  </si>
+  <si>
+    <t>after_battle</t>
+  </si>
+  <si>
+    <t>…これが私？どうしてこんなものが…私の記憶にはないけど…。</t>
+  </si>
+  <si>
+    <t>…Is this me? How could something like this exist? I don't remember it.</t>
   </si>
 </sst>
 </file>
@@ -428,14 +455,15 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.43"/>
-    <col customWidth="1" min="2" max="2" width="18.14"/>
-    <col customWidth="1" min="3" max="3" width="31.0"/>
+    <col customWidth="1" min="1" max="1" width="16.0"/>
+    <col customWidth="1" min="2" max="2" width="12.43"/>
+    <col customWidth="1" min="3" max="3" width="5.57"/>
     <col customWidth="1" min="4" max="4" width="19.29"/>
-    <col customWidth="1" min="5" max="5" width="16.14"/>
-    <col customWidth="1" min="6" max="6" width="8.86"/>
-    <col customWidth="1" min="7" max="8" width="7.14"/>
-    <col customWidth="1" min="9" max="9" width="42.14"/>
+    <col customWidth="1" min="5" max="5" width="15.14"/>
+    <col customWidth="1" min="6" max="6" width="5.43"/>
+    <col customWidth="1" min="7" max="7" width="7.29"/>
+    <col customWidth="1" min="8" max="8" width="7.14"/>
+    <col customWidth="1" min="9" max="9" width="61.14"/>
     <col customWidth="1" min="10" max="10" width="87.57"/>
     <col customWidth="1" min="11" max="11" width="42.57"/>
     <col customWidth="1" min="12" max="26" width="9.0"/>
@@ -485,8 +513,8 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1">
-        <f>MAX(H4:H1048580)</f>
-        <v>7</v>
+        <f>MAX(H4:H1048574)</f>
+        <v>9</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="3"/>
@@ -642,7 +670,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="5">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>18</v>
@@ -755,7 +783,7 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="5">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>25</v>
@@ -863,7 +891,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="5">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="I31" s="5" t="s">
         <v>28</v>
@@ -881,7 +909,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="5">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="I32" s="5" t="s">
         <v>30</v>
@@ -894,23 +922,27 @@
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="7" t="s">
-        <v>22</v>
-      </c>
+      <c r="D33" s="2"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="3"/>
+      <c r="H33" s="5">
+        <v>6.0</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="5" t="s">
-        <v>20</v>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="7" t="s">
+        <v>21</v>
       </c>
-      <c r="C34" s="1"/>
-      <c r="D34" s="2"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -920,7 +952,9 @@
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
+      <c r="B35" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
       <c r="E35" s="1"/>
@@ -951,13 +985,11 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
+      <c r="I37" s="9"/>
       <c r="J37" s="3"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -969,7 +1001,9 @@
       <c r="J38" s="3"/>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="1"/>
+      <c r="A39" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -988,35 +1022,35 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
-      <c r="H40" s="5">
-        <v>7.0</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>33</v>
-      </c>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="3"/>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
-      <c r="D41" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="D41" s="2"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="3"/>
+      <c r="H41" s="5">
+        <v>7.0</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="42" ht="12.75" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="2"/>
+      <c r="D42" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -1026,7 +1060,9 @@
     </row>
     <row r="43" ht="12.75" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
+      <c r="B43" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="C43" s="1"/>
       <c r="D43" s="2"/>
       <c r="E43" s="1"/>
@@ -1045,7 +1081,7 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-      <c r="I44" s="9"/>
+      <c r="I44" s="1"/>
       <c r="J44" s="3"/>
     </row>
     <row r="45" ht="12.75" customHeight="1">
@@ -1069,36 +1105,48 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-      <c r="I46" s="1"/>
+      <c r="I46" s="9"/>
       <c r="J46" s="3"/>
     </row>
     <row r="47" ht="12.75" customHeight="1">
-      <c r="A47" s="1"/>
+      <c r="A47" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="2"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="3"/>
+      <c r="H47" s="5">
+        <v>8.0</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="48" ht="12.75" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
-      <c r="D48" s="2"/>
+      <c r="D48" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
-      <c r="I48" s="9"/>
+      <c r="I48" s="1"/>
       <c r="J48" s="3"/>
     </row>
     <row r="49" ht="12.75" customHeight="1">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
+      <c r="B49" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="C49" s="1"/>
       <c r="D49" s="2"/>
       <c r="E49" s="1"/>
@@ -1129,7 +1177,7 @@
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
-      <c r="I51" s="1"/>
+      <c r="I51" s="9"/>
       <c r="J51" s="3"/>
     </row>
     <row r="52" ht="12.75" customHeight="1">
@@ -1145,7 +1193,9 @@
       <c r="J52" s="3"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" s="1"/>
+      <c r="A53" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="2"/>
@@ -1153,7 +1203,7 @@
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
+      <c r="I53" s="9"/>
       <c r="J53" s="3"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
@@ -1164,15 +1214,23 @@
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="3"/>
+      <c r="H54" s="5">
+        <v>9.0</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
-      <c r="D55" s="2"/>
+      <c r="D55" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -1182,7 +1240,9 @@
     </row>
     <row r="56" ht="12.75" customHeight="1">
       <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
+      <c r="B56" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="C56" s="1"/>
       <c r="D56" s="2"/>
       <c r="E56" s="1"/>
@@ -1201,7 +1261,7 @@
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
-      <c r="I57" s="9"/>
+      <c r="I57" s="1"/>
       <c r="J57" s="3"/>
     </row>
     <row r="58" ht="12.75" customHeight="1">
@@ -1213,7 +1273,7 @@
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
-      <c r="I58" s="9"/>
+      <c r="I58" s="1"/>
       <c r="J58" s="3"/>
     </row>
     <row r="59" ht="12.75" customHeight="1">
@@ -1225,7 +1285,7 @@
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
-      <c r="I59" s="9"/>
+      <c r="I59" s="1"/>
       <c r="J59" s="3"/>
     </row>
     <row r="60" ht="12.75" customHeight="1">
@@ -1297,7 +1357,7 @@
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
-      <c r="I65" s="1"/>
+      <c r="I65" s="9"/>
       <c r="J65" s="3"/>
     </row>
     <row r="66" ht="12.75" customHeight="1">
@@ -1369,7 +1429,7 @@
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
-      <c r="I71" s="9"/>
+      <c r="I71" s="1"/>
       <c r="J71" s="3"/>
     </row>
     <row r="72" ht="12.75" customHeight="1">
@@ -1417,7 +1477,7 @@
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
-      <c r="I75" s="1"/>
+      <c r="I75" s="9"/>
       <c r="J75" s="3"/>
     </row>
     <row r="76" ht="12.75" customHeight="1">
@@ -1465,7 +1525,7 @@
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
-      <c r="I79" s="1"/>
+      <c r="I79" s="9"/>
       <c r="J79" s="3"/>
     </row>
     <row r="80" ht="12.75" customHeight="1">
@@ -1477,7 +1537,7 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
-      <c r="I80" s="1"/>
+      <c r="I80" s="9"/>
       <c r="J80" s="3"/>
     </row>
     <row r="81" ht="12.75" customHeight="1">
@@ -1489,7 +1549,7 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
-      <c r="I81" s="9"/>
+      <c r="I81" s="1"/>
       <c r="J81" s="3"/>
     </row>
     <row r="82" ht="12.75" customHeight="1">
@@ -1501,7 +1561,7 @@
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
-      <c r="I82" s="1"/>
+      <c r="I82" s="9"/>
       <c r="J82" s="3"/>
     </row>
     <row r="83" ht="12.75" customHeight="1">
@@ -1537,7 +1597,7 @@
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
-      <c r="I85" s="9"/>
+      <c r="I85" s="1"/>
       <c r="J85" s="3"/>
     </row>
     <row r="86" ht="12.75" customHeight="1">
@@ -1549,7 +1609,7 @@
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
-      <c r="I86" s="9"/>
+      <c r="I86" s="1"/>
       <c r="J86" s="3"/>
     </row>
     <row r="87" ht="12.75" customHeight="1">
@@ -1561,7 +1621,7 @@
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
-      <c r="I87" s="1"/>
+      <c r="I87" s="9"/>
       <c r="J87" s="3"/>
     </row>
     <row r="88" ht="12.75" customHeight="1">
@@ -1573,7 +1633,7 @@
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
-      <c r="I88" s="9"/>
+      <c r="I88" s="1"/>
       <c r="J88" s="3"/>
     </row>
     <row r="89" ht="12.75" customHeight="1">
@@ -1681,7 +1741,7 @@
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
-      <c r="I97" s="1"/>
+      <c r="I97" s="10"/>
       <c r="J97" s="3"/>
     </row>
     <row r="98" ht="12.75" customHeight="1">
@@ -1693,7 +1753,7 @@
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
-      <c r="I98" s="1"/>
+      <c r="I98" s="10"/>
       <c r="J98" s="3"/>
     </row>
     <row r="99" ht="12.75" customHeight="1">
@@ -1705,7 +1765,7 @@
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
-      <c r="I99" s="9"/>
+      <c r="I99" s="1"/>
       <c r="J99" s="3"/>
     </row>
     <row r="100" ht="12.75" customHeight="1">
@@ -1753,7 +1813,7 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
-      <c r="I103" s="10"/>
+      <c r="I103" s="1"/>
       <c r="J103" s="3"/>
     </row>
     <row r="104" ht="12.75" customHeight="1">
@@ -1837,7 +1897,7 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
-      <c r="I110" s="10"/>
+      <c r="I110" s="1"/>
       <c r="J110" s="3"/>
     </row>
     <row r="111" ht="12.75" customHeight="1">
@@ -1845,7 +1905,7 @@
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
       <c r="D111" s="2"/>
-      <c r="E111" s="1"/>
+      <c r="E111" s="11"/>
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
@@ -1857,11 +1917,11 @@
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
       <c r="D112" s="2"/>
-      <c r="E112" s="1"/>
+      <c r="E112" s="11"/>
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
-      <c r="I112" s="1"/>
+      <c r="I112" s="12"/>
       <c r="J112" s="3"/>
     </row>
     <row r="113" ht="12.75" customHeight="1">
@@ -1873,7 +1933,7 @@
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
-      <c r="I113" s="1"/>
+      <c r="I113" s="10"/>
       <c r="J113" s="3"/>
     </row>
     <row r="114" ht="12.75" customHeight="1">
@@ -1885,7 +1945,7 @@
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
-      <c r="I114" s="1"/>
+      <c r="I114" s="10"/>
       <c r="J114" s="3"/>
     </row>
     <row r="115" ht="12.75" customHeight="1">
@@ -1917,7 +1977,7 @@
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
       <c r="D117" s="2"/>
-      <c r="E117" s="11"/>
+      <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
@@ -1929,11 +1989,11 @@
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
       <c r="D118" s="2"/>
-      <c r="E118" s="11"/>
+      <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
-      <c r="I118" s="12"/>
+      <c r="I118" s="1"/>
       <c r="J118" s="3"/>
     </row>
     <row r="119" ht="12.75" customHeight="1">
@@ -1945,7 +2005,7 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
-      <c r="I119" s="10"/>
+      <c r="I119" s="1"/>
       <c r="J119" s="3"/>
     </row>
     <row r="120" ht="12.75" customHeight="1">
@@ -1953,11 +2013,11 @@
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
       <c r="D120" s="2"/>
-      <c r="E120" s="1"/>
+      <c r="E120" s="11"/>
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
-      <c r="I120" s="10"/>
+      <c r="I120" s="1"/>
       <c r="J120" s="3"/>
     </row>
     <row r="121" ht="12.75" customHeight="1">
@@ -1965,11 +2025,11 @@
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
       <c r="D121" s="2"/>
-      <c r="E121" s="1"/>
+      <c r="E121" s="11"/>
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
-      <c r="I121" s="1"/>
+      <c r="I121" s="10"/>
       <c r="J121" s="3"/>
     </row>
     <row r="122" ht="12.75" customHeight="1">
@@ -1977,7 +2037,7 @@
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
       <c r="D122" s="2"/>
-      <c r="E122" s="1"/>
+      <c r="E122" s="11"/>
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
@@ -2049,11 +2109,11 @@
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
       <c r="D128" s="2"/>
-      <c r="E128" s="11"/>
+      <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
-      <c r="I128" s="1"/>
+      <c r="I128" s="10"/>
       <c r="J128" s="3"/>
     </row>
     <row r="129" ht="12.75" customHeight="1">
@@ -2097,7 +2157,7 @@
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
       <c r="D132" s="2"/>
-      <c r="E132" s="11"/>
+      <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
@@ -2109,11 +2169,11 @@
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
       <c r="D133" s="2"/>
-      <c r="E133" s="11"/>
+      <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
-      <c r="I133" s="10"/>
+      <c r="I133" s="1"/>
       <c r="J133" s="3"/>
     </row>
     <row r="134" ht="12.75" customHeight="1">
@@ -2125,11 +2185,11 @@
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
-      <c r="I134" s="10"/>
+      <c r="I134" s="1"/>
       <c r="J134" s="3"/>
     </row>
     <row r="135" ht="12.75" customHeight="1">
-      <c r="A135" s="1"/>
+      <c r="A135" s="11"/>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
       <c r="D135" s="2"/>
@@ -2157,7 +2217,7 @@
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
       <c r="D137" s="2"/>
-      <c r="E137" s="1"/>
+      <c r="E137" s="11"/>
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
@@ -2197,11 +2257,11 @@
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
-      <c r="I140" s="1"/>
+      <c r="I140" s="10"/>
       <c r="J140" s="3"/>
     </row>
     <row r="141" ht="12.75" customHeight="1">
-      <c r="A141" s="11"/>
+      <c r="A141" s="1"/>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
@@ -2209,7 +2269,7 @@
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
-      <c r="I141" s="1"/>
+      <c r="I141" s="10"/>
       <c r="J141" s="3"/>
     </row>
     <row r="142" ht="12.75" customHeight="1">
@@ -2221,7 +2281,7 @@
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
-      <c r="I142" s="1"/>
+      <c r="I142" s="10"/>
       <c r="J142" s="3"/>
     </row>
     <row r="143" ht="12.75" customHeight="1">
@@ -2229,11 +2289,11 @@
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
-      <c r="E143" s="11"/>
+      <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
-      <c r="I143" s="1"/>
+      <c r="I143" s="10"/>
       <c r="J143" s="3"/>
     </row>
     <row r="144" ht="12.75" customHeight="1">
@@ -2245,7 +2305,7 @@
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
-      <c r="I144" s="1"/>
+      <c r="I144" s="10"/>
       <c r="J144" s="3"/>
     </row>
     <row r="145" ht="12.75" customHeight="1">
@@ -2255,9 +2315,9 @@
       <c r="D145" s="2"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
-      <c r="G145" s="1"/>
+      <c r="G145" s="9"/>
       <c r="H145" s="1"/>
-      <c r="I145" s="1"/>
+      <c r="I145" s="10"/>
       <c r="J145" s="3"/>
     </row>
     <row r="146" ht="12.75" customHeight="1">
@@ -2305,7 +2365,7 @@
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
-      <c r="I149" s="10"/>
+      <c r="I149" s="9"/>
       <c r="J149" s="3"/>
     </row>
     <row r="150" ht="12.75" customHeight="1">
@@ -2317,7 +2377,7 @@
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
-      <c r="I150" s="10"/>
+      <c r="I150" s="9"/>
       <c r="J150" s="3"/>
     </row>
     <row r="151" ht="12.75" customHeight="1">
@@ -2327,7 +2387,7 @@
       <c r="D151" s="2"/>
       <c r="E151" s="1"/>
       <c r="F151" s="1"/>
-      <c r="G151" s="9"/>
+      <c r="G151" s="1"/>
       <c r="H151" s="1"/>
       <c r="I151" s="10"/>
       <c r="J151" s="3"/>
@@ -2337,11 +2397,11 @@
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
       <c r="D152" s="2"/>
-      <c r="E152" s="1"/>
+      <c r="E152" s="11"/>
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
-      <c r="I152" s="10"/>
+      <c r="I152" s="1"/>
       <c r="J152" s="3"/>
     </row>
     <row r="153" ht="12.75" customHeight="1">
@@ -2353,7 +2413,7 @@
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
-      <c r="I153" s="10"/>
+      <c r="I153" s="1"/>
       <c r="J153" s="3"/>
     </row>
     <row r="154" ht="12.75" customHeight="1">
@@ -2365,7 +2425,7 @@
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
-      <c r="I154" s="10"/>
+      <c r="I154" s="1"/>
       <c r="J154" s="3"/>
     </row>
     <row r="155" ht="12.75" customHeight="1">
@@ -2377,7 +2437,7 @@
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
-      <c r="I155" s="9"/>
+      <c r="I155" s="1"/>
       <c r="J155" s="3"/>
     </row>
     <row r="156" ht="12.75" customHeight="1">
@@ -2389,7 +2449,7 @@
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
-      <c r="I156" s="9"/>
+      <c r="I156" s="1"/>
       <c r="J156" s="3"/>
     </row>
     <row r="157" ht="12.75" customHeight="1">
@@ -2401,7 +2461,7 @@
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
-      <c r="I157" s="10"/>
+      <c r="I157" s="1"/>
       <c r="J157" s="3"/>
     </row>
     <row r="158" ht="12.75" customHeight="1">
@@ -2409,7 +2469,7 @@
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
       <c r="D158" s="2"/>
-      <c r="E158" s="11"/>
+      <c r="E158" s="1"/>
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
@@ -12496,78 +12556,6 @@
       <c r="I998" s="1"/>
       <c r="J998" s="3"/>
     </row>
-    <row r="999" ht="12.75" customHeight="1">
-      <c r="A999" s="1"/>
-      <c r="B999" s="1"/>
-      <c r="C999" s="1"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="1"/>
-      <c r="F999" s="1"/>
-      <c r="G999" s="1"/>
-      <c r="H999" s="1"/>
-      <c r="I999" s="1"/>
-      <c r="J999" s="3"/>
-    </row>
-    <row r="1000" ht="12.75" customHeight="1">
-      <c r="A1000" s="1"/>
-      <c r="B1000" s="1"/>
-      <c r="C1000" s="1"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="1"/>
-      <c r="F1000" s="1"/>
-      <c r="G1000" s="1"/>
-      <c r="H1000" s="1"/>
-      <c r="I1000" s="1"/>
-      <c r="J1000" s="3"/>
-    </row>
-    <row r="1001" ht="12.75" customHeight="1">
-      <c r="A1001" s="1"/>
-      <c r="B1001" s="1"/>
-      <c r="C1001" s="1"/>
-      <c r="D1001" s="2"/>
-      <c r="E1001" s="1"/>
-      <c r="F1001" s="1"/>
-      <c r="G1001" s="1"/>
-      <c r="H1001" s="1"/>
-      <c r="I1001" s="1"/>
-      <c r="J1001" s="3"/>
-    </row>
-    <row r="1002" ht="12.75" customHeight="1">
-      <c r="A1002" s="1"/>
-      <c r="B1002" s="1"/>
-      <c r="C1002" s="1"/>
-      <c r="D1002" s="2"/>
-      <c r="E1002" s="1"/>
-      <c r="F1002" s="1"/>
-      <c r="G1002" s="1"/>
-      <c r="H1002" s="1"/>
-      <c r="I1002" s="1"/>
-      <c r="J1002" s="3"/>
-    </row>
-    <row r="1003" ht="12.75" customHeight="1">
-      <c r="A1003" s="1"/>
-      <c r="B1003" s="1"/>
-      <c r="C1003" s="1"/>
-      <c r="D1003" s="2"/>
-      <c r="E1003" s="1"/>
-      <c r="F1003" s="1"/>
-      <c r="G1003" s="1"/>
-      <c r="H1003" s="1"/>
-      <c r="I1003" s="1"/>
-      <c r="J1003" s="3"/>
-    </row>
-    <row r="1004" ht="12.75" customHeight="1">
-      <c r="A1004" s="1"/>
-      <c r="B1004" s="1"/>
-      <c r="C1004" s="1"/>
-      <c r="D1004" s="2"/>
-      <c r="E1004" s="1"/>
-      <c r="F1004" s="1"/>
-      <c r="G1004" s="1"/>
-      <c r="H1004" s="1"/>
-      <c r="I1004" s="1"/>
-      <c r="J1004" s="3"/>
-    </row>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>